<commit_message>
Connect unit with chassis
</commit_message>
<xml_diff>
--- a/TspuWebPortal/Development/unsafe_uploads/Test_Vedomost.xlsx
+++ b/TspuWebPortal/Development/unsafe_uploads/Test_Vedomost.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="949" uniqueCount="217">
   <si>
     <t>Серийный номер</t>
   </si>
@@ -665,6 +665,21 @@
   </si>
   <si>
     <t>материнская плата</t>
+  </si>
+  <si>
+    <t>ЦОД-1</t>
+  </si>
+  <si>
+    <t>ЦОД</t>
+  </si>
+  <si>
+    <t>Помещение</t>
+  </si>
+  <si>
+    <t>Ряд</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -748,11 +763,12 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1035,24 +1051,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M66"/>
+  <dimension ref="A1:O66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="N49" sqref="N49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64" customWidth="1"/>
+    <col min="3" max="3" width="66.85546875" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="24.28515625" customWidth="1"/>
     <col min="6" max="6" width="9.140625" customWidth="1"/>
     <col min="7" max="7" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="51.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1090,10 +1109,16 @@
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>13</v>
       </c>
@@ -1111,8 +1136,8 @@
         <v>16</v>
       </c>
       <c r="G2" s="3"/>
-      <c r="H2" s="3">
-        <v>1</v>
+      <c r="H2" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>195</v>
@@ -1127,10 +1152,16 @@
         <v>2020</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N2" s="3">
+        <v>404</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -1160,10 +1191,16 @@
         <v>2020</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N3" s="3">
+        <v>404</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>25</v>
       </c>
@@ -1193,10 +1230,16 @@
         <v>2020</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N4" s="3">
+        <v>404</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>28</v>
       </c>
@@ -1226,10 +1269,16 @@
         <v>2020</v>
       </c>
       <c r="M5" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N5" s="3">
+        <v>404</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
@@ -1258,9 +1307,17 @@
       <c r="L6" s="3">
         <v>2021</v>
       </c>
-      <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M6" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="N6" s="3">
+        <v>404</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>36</v>
       </c>
@@ -1289,9 +1346,17 @@
       <c r="L7" s="3">
         <v>2021</v>
       </c>
-      <c r="M7" s="3"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M7" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="N7" s="3">
+        <v>404</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>38</v>
       </c>
@@ -1320,9 +1385,17 @@
       <c r="L8" s="3">
         <v>2021</v>
       </c>
-      <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M8" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="N8" s="3">
+        <v>404</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>40</v>
       </c>
@@ -1351,9 +1424,17 @@
       <c r="L9" s="3">
         <v>2021</v>
       </c>
-      <c r="M9" s="3"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M9" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="N9" s="3">
+        <v>404</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
@@ -1382,9 +1463,17 @@
       <c r="L10" s="3">
         <v>2021</v>
       </c>
-      <c r="M10" s="3"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M10" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="N10" s="3">
+        <v>404</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>44</v>
       </c>
@@ -1413,9 +1502,17 @@
       <c r="L11" s="3">
         <v>2021</v>
       </c>
-      <c r="M11" s="3"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M11" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="N11" s="3">
+        <v>404</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>46</v>
       </c>
@@ -1449,10 +1546,16 @@
         <v>2020</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N12" s="3">
+        <v>404</v>
+      </c>
+      <c r="O12" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>51</v>
       </c>
@@ -1482,10 +1585,16 @@
         <v>2020</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N13" s="3">
+        <v>404</v>
+      </c>
+      <c r="O13" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>53</v>
       </c>
@@ -1515,10 +1624,16 @@
         <v>2020</v>
       </c>
       <c r="M14" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N14" s="3">
+        <v>404</v>
+      </c>
+      <c r="O14" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>55</v>
       </c>
@@ -1548,10 +1663,16 @@
         <v>2020</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N15" s="3">
+        <v>404</v>
+      </c>
+      <c r="O15" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>57</v>
       </c>
@@ -1585,10 +1706,16 @@
         <v>2020</v>
       </c>
       <c r="M16" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N16" s="3">
+        <v>404</v>
+      </c>
+      <c r="O16" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>60</v>
       </c>
@@ -1618,10 +1745,16 @@
         <v>2020</v>
       </c>
       <c r="M17" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N17" s="3">
+        <v>404</v>
+      </c>
+      <c r="O17" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>62</v>
       </c>
@@ -1651,10 +1784,16 @@
         <v>2020</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N18" s="3">
+        <v>404</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>64</v>
       </c>
@@ -1684,10 +1823,16 @@
         <v>2020</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N19" s="3">
+        <v>404</v>
+      </c>
+      <c r="O19" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>68</v>
       </c>
@@ -1721,10 +1866,16 @@
         <v>2020</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N20" s="3">
+        <v>404</v>
+      </c>
+      <c r="O20" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>70</v>
       </c>
@@ -1754,10 +1905,16 @@
         <v>2020</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N21" s="3">
+        <v>404</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>72</v>
       </c>
@@ -1787,10 +1944,16 @@
         <v>2020</v>
       </c>
       <c r="M22" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N22" s="3">
+        <v>404</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>74</v>
       </c>
@@ -1820,10 +1983,16 @@
         <v>2020</v>
       </c>
       <c r="M23" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N23" s="3">
+        <v>404</v>
+      </c>
+      <c r="O23" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>76</v>
       </c>
@@ -1857,10 +2026,16 @@
         <v>2020</v>
       </c>
       <c r="M24" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N24" s="3">
+        <v>404</v>
+      </c>
+      <c r="O24" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>78</v>
       </c>
@@ -1890,10 +2065,16 @@
         <v>2020</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N25" s="3">
+        <v>404</v>
+      </c>
+      <c r="O25" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>80</v>
       </c>
@@ -1923,10 +2104,16 @@
         <v>2020</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N26" s="3">
+        <v>404</v>
+      </c>
+      <c r="O26" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>82</v>
       </c>
@@ -1956,10 +2143,16 @@
         <v>2020</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N27" s="3">
+        <v>404</v>
+      </c>
+      <c r="O27" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>84</v>
       </c>
@@ -1993,10 +2186,16 @@
         <v>2020</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N28" s="3">
+        <v>404</v>
+      </c>
+      <c r="O28" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>87</v>
       </c>
@@ -2026,10 +2225,16 @@
         <v>2020</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N29" s="3">
+        <v>404</v>
+      </c>
+      <c r="O29" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>89</v>
       </c>
@@ -2059,10 +2264,16 @@
         <v>2020</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N30" s="3">
+        <v>404</v>
+      </c>
+      <c r="O30" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>91</v>
       </c>
@@ -2092,10 +2303,16 @@
         <v>2020</v>
       </c>
       <c r="M31" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N31" s="3">
+        <v>404</v>
+      </c>
+      <c r="O31" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>93</v>
       </c>
@@ -2129,10 +2346,16 @@
         <v>2020</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N32" s="3">
+        <v>404</v>
+      </c>
+      <c r="O32" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>96</v>
       </c>
@@ -2162,10 +2385,16 @@
         <v>2020</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N33" s="3">
+        <v>404</v>
+      </c>
+      <c r="O33" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>98</v>
       </c>
@@ -2195,10 +2424,16 @@
         <v>2020</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N34" s="3">
+        <v>404</v>
+      </c>
+      <c r="O34" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>100</v>
       </c>
@@ -2228,10 +2463,16 @@
         <v>2020</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N35" s="3">
+        <v>404</v>
+      </c>
+      <c r="O35" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>102</v>
       </c>
@@ -2265,10 +2506,16 @@
         <v>2020</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N36" s="3">
+        <v>404</v>
+      </c>
+      <c r="O36" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>105</v>
       </c>
@@ -2298,10 +2545,16 @@
         <v>2020</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N37" s="3">
+        <v>404</v>
+      </c>
+      <c r="O37" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>107</v>
       </c>
@@ -2331,10 +2584,16 @@
         <v>2020</v>
       </c>
       <c r="M38" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N38" s="3">
+        <v>404</v>
+      </c>
+      <c r="O38" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>109</v>
       </c>
@@ -2364,10 +2623,16 @@
         <v>2020</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N39" s="3">
+        <v>404</v>
+      </c>
+      <c r="O39" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>111</v>
       </c>
@@ -2401,10 +2666,16 @@
         <v>2020</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N40" s="3">
+        <v>404</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>115</v>
       </c>
@@ -2434,10 +2705,16 @@
         <v>2020</v>
       </c>
       <c r="M41" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N41" s="3">
+        <v>404</v>
+      </c>
+      <c r="O41" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>117</v>
       </c>
@@ -2467,10 +2744,16 @@
         <v>2020</v>
       </c>
       <c r="M42" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N42" s="3">
+        <v>404</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>119</v>
       </c>
@@ -2500,10 +2783,16 @@
         <v>2020</v>
       </c>
       <c r="M43" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N43" s="3">
+        <v>404</v>
+      </c>
+      <c r="O43" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>121</v>
       </c>
@@ -2537,10 +2826,16 @@
         <v>2020</v>
       </c>
       <c r="M44" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N44" s="3">
+        <v>404</v>
+      </c>
+      <c r="O44" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>123</v>
       </c>
@@ -2570,10 +2865,16 @@
         <v>2020</v>
       </c>
       <c r="M45" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N45" s="3">
+        <v>404</v>
+      </c>
+      <c r="O45" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>125</v>
       </c>
@@ -2603,10 +2904,16 @@
         <v>2020</v>
       </c>
       <c r="M46" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N46" s="3">
+        <v>404</v>
+      </c>
+      <c r="O46" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>127</v>
       </c>
@@ -2636,10 +2943,16 @@
         <v>2020</v>
       </c>
       <c r="M47" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N47" s="3">
+        <v>404</v>
+      </c>
+      <c r="O47" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>129</v>
       </c>
@@ -2673,10 +2986,16 @@
         <v>2020</v>
       </c>
       <c r="M48" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N48" s="3">
+        <v>404</v>
+      </c>
+      <c r="O48" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>131</v>
       </c>
@@ -2706,10 +3025,16 @@
         <v>2020</v>
       </c>
       <c r="M49" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N49" s="3">
+        <v>404</v>
+      </c>
+      <c r="O49" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>133</v>
       </c>
@@ -2739,10 +3064,16 @@
         <v>2020</v>
       </c>
       <c r="M50" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N50" s="3">
+        <v>404</v>
+      </c>
+      <c r="O50" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>135</v>
       </c>
@@ -2772,10 +3103,16 @@
         <v>2020</v>
       </c>
       <c r="M51" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N51" s="3">
+        <v>404</v>
+      </c>
+      <c r="O51" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>137</v>
       </c>
@@ -2805,10 +3142,16 @@
         <v>2019</v>
       </c>
       <c r="M52" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N52" s="3">
+        <v>404</v>
+      </c>
+      <c r="O52" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>140</v>
       </c>
@@ -2836,10 +3179,16 @@
         <v>2020</v>
       </c>
       <c r="M53" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N53" s="3">
+        <v>404</v>
+      </c>
+      <c r="O53" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>143</v>
       </c>
@@ -2859,16 +3208,24 @@
       <c r="I54" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="J54" s="3"/>
+      <c r="J54" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="K54" s="3"/>
       <c r="L54" s="3">
         <v>2020</v>
       </c>
       <c r="M54" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N54" s="3">
+        <v>404</v>
+      </c>
+      <c r="O54" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>146</v>
       </c>
@@ -2904,10 +3261,16 @@
         <v>2021</v>
       </c>
       <c r="M55" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N55" s="3">
+        <v>404</v>
+      </c>
+      <c r="O55" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>152</v>
       </c>
@@ -2937,10 +3300,16 @@
         <v>2021</v>
       </c>
       <c r="M56" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N56" s="3">
+        <v>404</v>
+      </c>
+      <c r="O56" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>155</v>
       </c>
@@ -2970,10 +3339,16 @@
         <v>2021</v>
       </c>
       <c r="M57" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N57" s="3">
+        <v>404</v>
+      </c>
+      <c r="O57" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>157</v>
       </c>
@@ -3005,10 +3380,16 @@
         <v>2020</v>
       </c>
       <c r="M58" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N58" s="3">
+        <v>404</v>
+      </c>
+      <c r="O58" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>161</v>
       </c>
@@ -3040,10 +3421,16 @@
         <v>2020</v>
       </c>
       <c r="M59" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N59" s="3">
+        <v>404</v>
+      </c>
+      <c r="O59" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>166</v>
       </c>
@@ -3075,10 +3462,16 @@
         <v>2020</v>
       </c>
       <c r="M60" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N60" s="3">
+        <v>404</v>
+      </c>
+      <c r="O60" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>170</v>
       </c>
@@ -3110,10 +3503,16 @@
         <v>2020</v>
       </c>
       <c r="M61" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N61" s="3">
+        <v>404</v>
+      </c>
+      <c r="O61" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>173</v>
       </c>
@@ -3145,10 +3544,16 @@
         <v>2020</v>
       </c>
       <c r="M62" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N62" s="3">
+        <v>404</v>
+      </c>
+      <c r="O62" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>176</v>
       </c>
@@ -3180,10 +3585,16 @@
         <v>2020</v>
       </c>
       <c r="M63" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N63" s="3">
+        <v>404</v>
+      </c>
+      <c r="O63" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>180</v>
       </c>
@@ -3215,10 +3626,16 @@
         <v>2020</v>
       </c>
       <c r="M64" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N64" s="3">
+        <v>404</v>
+      </c>
+      <c r="O64" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>183</v>
       </c>
@@ -3250,10 +3667,16 @@
         <v>2020</v>
       </c>
       <c r="M65" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
+        <v>212</v>
+      </c>
+      <c r="N65" s="3">
+        <v>404</v>
+      </c>
+      <c r="O65" s="4" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>188</v>
       </c>
@@ -3287,7 +3710,13 @@
         <v>209</v>
       </c>
       <c r="M66" s="3" t="s">
-        <v>19</v>
+        <v>212</v>
+      </c>
+      <c r="N66" s="3">
+        <v>404</v>
+      </c>
+      <c r="O66" s="4" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>